<commit_message>
Updated on 11.04am 11st Feb 2015 from SR PC
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>project-01.jpg -&gt; change to for sale</t>
   </si>
@@ -99,6 +99,14 @@
   </si>
   <si>
     <t>Result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -225,9 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -237,11 +242,50 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -534,7 +578,7 @@
   <dimension ref="A3:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -544,163 +588,203 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -710,6 +794,14 @@
     <mergeCell ref="A22:A23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C4:C23">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated on 03.11pm 11st Feb 2015 from cjoo pc
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="20415" windowHeight="7770"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>project-01.jpg -&gt; change to for sale</t>
   </si>
@@ -108,6 +108,9 @@
   <si>
     <t>f</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -118,14 +121,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -134,7 +137,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -249,14 +252,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -268,20 +264,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,14 +559,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -624,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -633,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -660,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -795,10 +777,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C4:C23">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",C4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -813,7 +795,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -826,7 +808,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 12.12pm 12nd Feb 2015 from SR
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="20415" windowHeight="7770"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -121,14 +121,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -137,7 +137,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -559,14 +559,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="52.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -633,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -795,7 +795,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -808,7 +808,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 11.18am 13th Feb 2015 from SR
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -673,7 +673,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -682,7 +682,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -700,7 +700,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -709,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -727,7 +727,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -736,7 +736,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -745,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3">

</xml_diff>

<commit_message>
Updated on 1.42am 15th Feb 2015 from cjoo pc
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="20415" windowHeight="7770"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>project-01.jpg -&gt; change to for sale</t>
   </si>
@@ -102,15 +102,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t</t>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>completed</t>
   </si>
 </sst>
 </file>
@@ -121,14 +116,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -137,7 +132,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -157,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,60 +175,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -252,7 +201,35 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -559,106 +536,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="2" max="2" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -666,122 +632,106 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="C12:C21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C4:C23">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="T">
-      <formula>NOT(ISERROR(SEARCH("T",C4)))</formula>
+  <conditionalFormatting sqref="C11 C22:C23">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",C4)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -795,7 +745,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -808,7 +758,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 18th Feb 09.41pm from SR
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="20415" windowHeight="7770"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>project-01.jpg -&gt; change to for sale</t>
   </si>
@@ -106,6 +106,58 @@
   </si>
   <si>
     <t>completed</t>
+  </si>
+  <si>
+    <t>Inbetween -&gt; 1600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add tesitimonial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Summer island series (pair) 400x400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Gallery -&gt; 1300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message : only the left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫페이지에 For sale 이랑 Sold랑 separate 하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫페이지 3rd background image 바꾸기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모바일-&gt; gallery 들 사진 확대 안하게 하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모바일-&gt; gallery에서 arrow 위치 조정하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Craig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">매인페이지에 For sale 밑에만 글씨를 써라 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콘택트 사진은 새로 주겠다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kate Cambell 사진 모바일에서 짤리는거 수정하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -116,14 +168,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -132,7 +184,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -201,14 +253,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -220,27 +265,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -534,17 +558,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C23"/>
+  <dimension ref="A3:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" customWidth="1"/>
+    <col min="2" max="2" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -714,6 +738,69 @@
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="B42" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -727,11 +814,11 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C11 C22:C23">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="T">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="T">
       <formula>NOT(ISERROR(SEARCH("T",C11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -745,7 +832,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -758,7 +845,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated on 12.24pm 24th Feb 2015 from SR
</commit_message>
<xml_diff>
--- a/SR.xlsx
+++ b/SR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>project-01.jpg -&gt; change to for sale</t>
   </si>
@@ -157,6 +157,10 @@
   </si>
   <si>
     <t>Kate Cambell 사진 모바일에서 짤리는거 수정하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -560,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -744,61 +748,88 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>30</v>
       </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
         <v>28</v>
       </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
         <v>29</v>
       </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="B32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="B33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="B35" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="B36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="B38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="B39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="B42" t="s">
         <v>38</v>
       </c>

</xml_diff>